<commit_message>
DRC fixes after changing via size. fixed too small cap in PSU.
</commit_message>
<xml_diff>
--- a/CM5IO/RPI-CM5IO-R2-Gerber050325/Required_impedance_control.xlsx
+++ b/CM5IO/RPI-CM5IO-R2-Gerber050325/Required_impedance_control.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Distaff-GM\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Elektronika Schematy\KiCad\IARC-RPi_CM5_drone_platform\CM5IO\RPI-CM5IO-R2-Gerber050325\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3806B1-2207-449D-8F81-66E3C4AE238D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC51E02D-FF17-455C-96AE-F9A5DE46B977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,6 +358,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -370,7 +371,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,22 +393,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>6062</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>242455</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>66457</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>212243</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>121209</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB3F530E-6541-8FD1-41B0-EEF5EA84D255}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51294D86-A45F-938B-1093-D083399BA923}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -424,8 +424,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9548380" y="376052"/>
-          <a:ext cx="12740120" cy="16333178"/>
+          <a:off x="9525000" y="2274794"/>
+          <a:ext cx="7249537" cy="9354856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>229616</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>131176</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89617C53-10DA-BBA5-D088-6E345A003884}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9542318" y="294409"/>
+          <a:ext cx="7278116" cy="9240540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -697,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -721,10 +765,10 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
@@ -745,11 +789,11 @@
       <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="12">
         <v>4.25</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13">
+      <c r="E2" s="13"/>
+      <c r="F2" s="9">
         <v>5.9055</v>
       </c>
       <c r="G2" s="6">
@@ -767,11 +811,11 @@
       <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="12">
         <v>4.25</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13">
+      <c r="E3" s="13"/>
+      <c r="F3" s="9">
         <v>5.9055</v>
       </c>
       <c r="G3" s="6">
@@ -789,11 +833,11 @@
       <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="12">
         <v>6.6</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13">
+      <c r="E4" s="13"/>
+      <c r="F4" s="9">
         <v>9.9605999999999995</v>
       </c>
       <c r="G4" s="6">
@@ -811,11 +855,11 @@
       <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="12">
         <v>6.6</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13">
+      <c r="E5" s="13"/>
+      <c r="F5" s="9">
         <v>9.9605999999999995</v>
       </c>
       <c r="G5" s="6">

</xml_diff>

<commit_message>
Add PCIe connector. Fix some clearance violations.
</commit_message>
<xml_diff>
--- a/CM5IO/RPI-CM5IO-R2-Gerber050325/Required_impedance_control.xlsx
+++ b/CM5IO/RPI-CM5IO-R2-Gerber050325/Required_impedance_control.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Elektronika Schematy\KiCad\IARC-RPi_CM5_drone_platform\CM5IO\RPI-CM5IO-R2-Gerber050325\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC51E02D-FF17-455C-96AE-F9A5DE46B977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDAE6FB-0894-4206-9B61-ACC8F2EF271C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -394,21 +394,21 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>212243</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>121209</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>51954</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>175477</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51294D86-A45F-938B-1093-D083399BA923}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A59EF08A-0CDD-853F-14A7-13DB541955A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -424,8 +424,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9525000" y="2274794"/>
-          <a:ext cx="7249537" cy="9354856"/>
+          <a:off x="9542318" y="294409"/>
+          <a:ext cx="9525000" cy="11951841"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -436,23 +436,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>51953</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>229616</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>131176</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>36543</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89617C53-10DA-BBA5-D088-6E345A003884}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E46547B-AD72-D858-0078-88EAA1B17B17}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -468,8 +468,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9542318" y="294409"/>
-          <a:ext cx="7278116" cy="9240540"/>
+          <a:off x="19067317" y="294409"/>
+          <a:ext cx="9682771" cy="11949546"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -742,7 +742,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+      <selection activeCell="AM17" sqref="AM17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>